<commit_message>
venga for the lolz
</commit_message>
<xml_diff>
--- a/datos/zsdr159/zsdr159_60_2018_12_2019_12.XLSX
+++ b/datos/zsdr159/zsdr159_60_2018_12_2019_12.XLSX
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pelishka\Documents\repositorios\cuervo\datos\zsdr159\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F64451C-10E4-44C4-BED4-A1D486855511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21855" windowHeight="14940"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="267">
   <si>
     <t>0330</t>
   </si>
@@ -25,7 +42,7 @@
     <t>Intercompañías</t>
   </si>
   <si>
-    <t> /4500419195</t>
+    <t>/4500419195</t>
   </si>
   <si>
     <t>4700812035</t>
@@ -91,7 +108,7 @@
     <t>GIN.OSO.NEG.38% 12/1L</t>
   </si>
   <si>
-    <t> /4500419176</t>
+    <t>/4500419176</t>
   </si>
   <si>
     <t>4700812646</t>
@@ -109,7 +126,7 @@
     <t>0491420710</t>
   </si>
   <si>
-    <t> /4500419650</t>
+    <t>/4500419650</t>
   </si>
   <si>
     <t>4700813680</t>
@@ -121,7 +138,7 @@
     <t>0491421729</t>
   </si>
   <si>
-    <t> /4500420342</t>
+    <t>/4500420342</t>
   </si>
   <si>
     <t>4700816027</t>
@@ -133,7 +150,7 @@
     <t>0491423161</t>
   </si>
   <si>
-    <t> /4500420332</t>
+    <t>/4500420332</t>
   </si>
   <si>
     <t>4700816055</t>
@@ -148,7 +165,7 @@
     <t>0491423401</t>
   </si>
   <si>
-    <t> /4500420364</t>
+    <t>/4500420364</t>
   </si>
   <si>
     <t>4700816057</t>
@@ -166,7 +183,7 @@
     <t>0491423227</t>
   </si>
   <si>
-    <t> /4500413265</t>
+    <t>/4500413265</t>
   </si>
   <si>
     <t>4700816076</t>
@@ -178,7 +195,7 @@
     <t>0491423343</t>
   </si>
   <si>
-    <t> /4500420366</t>
+    <t>/4500420366</t>
   </si>
   <si>
     <t>4700816190</t>
@@ -202,7 +219,7 @@
     <t>0491423413</t>
   </si>
   <si>
-    <t> /4500414942</t>
+    <t>/4500414942</t>
   </si>
   <si>
     <t>4700819262</t>
@@ -214,7 +231,7 @@
     <t>0491424262</t>
   </si>
   <si>
-    <t> /4500421286</t>
+    <t>/4500421286</t>
   </si>
   <si>
     <t>4700819933</t>
@@ -229,7 +246,7 @@
     <t>C08</t>
   </si>
   <si>
-    <t> /4500422353</t>
+    <t>/4500422353</t>
   </si>
   <si>
     <t>4700824501</t>
@@ -253,7 +270,7 @@
     <t>0491426992</t>
   </si>
   <si>
-    <t> /4500423794</t>
+    <t>/4500423794</t>
   </si>
   <si>
     <t>4700826721</t>
@@ -265,7 +282,7 @@
     <t>0491428175</t>
   </si>
   <si>
-    <t> /4500425612</t>
+    <t>/4500425612</t>
   </si>
   <si>
     <t>4700830368</t>
@@ -277,7 +294,7 @@
     <t>0491429819</t>
   </si>
   <si>
-    <t> /4500428256</t>
+    <t>/4500428256</t>
   </si>
   <si>
     <t>4700837281</t>
@@ -307,7 +324,7 @@
     <t>GIN.OSO.NEG.38% 12/1L 19</t>
   </si>
   <si>
-    <t> /4500429731</t>
+    <t>/4500429731</t>
   </si>
   <si>
     <t>4700840492</t>
@@ -325,7 +342,7 @@
     <t>0491434560</t>
   </si>
   <si>
-    <t> /4500429967</t>
+    <t>/4500429967</t>
   </si>
   <si>
     <t>4700840876</t>
@@ -337,7 +354,7 @@
     <t>0491434628</t>
   </si>
   <si>
-    <t> /4500430155</t>
+    <t>/4500430155</t>
   </si>
   <si>
     <t>4700841101</t>
@@ -349,7 +366,7 @@
     <t>0491434816</t>
   </si>
   <si>
-    <t> /4500430840</t>
+    <t>/4500430840</t>
   </si>
   <si>
     <t>4700844642</t>
@@ -361,7 +378,7 @@
     <t>0491436602</t>
   </si>
   <si>
-    <t> /4500432227</t>
+    <t>/4500432227</t>
   </si>
   <si>
     <t>4700847516</t>
@@ -379,7 +396,7 @@
     <t>0491439126</t>
   </si>
   <si>
-    <t> /4500432069</t>
+    <t>/4500432069</t>
   </si>
   <si>
     <t>4700847552</t>
@@ -391,7 +408,7 @@
     <t>0491438637</t>
   </si>
   <si>
-    <t> /4500431786</t>
+    <t>/4500431786</t>
   </si>
   <si>
     <t>4700847733</t>
@@ -409,7 +426,7 @@
     <t>0491438729</t>
   </si>
   <si>
-    <t> /4500433182</t>
+    <t>/4500433182</t>
   </si>
   <si>
     <t>4700849201</t>
@@ -427,7 +444,7 @@
     <t>0491439559</t>
   </si>
   <si>
-    <t> /4500433353</t>
+    <t>/4500433353</t>
   </si>
   <si>
     <t>4700849564</t>
@@ -439,7 +456,7 @@
     <t>0491439607</t>
   </si>
   <si>
-    <t> /4500433448</t>
+    <t>/4500433448</t>
   </si>
   <si>
     <t>4700849822</t>
@@ -451,7 +468,7 @@
     <t>0491439745</t>
   </si>
   <si>
-    <t> /4500433467</t>
+    <t>/4500433467</t>
   </si>
   <si>
     <t>4700849837</t>
@@ -463,7 +480,7 @@
     <t>0491439825</t>
   </si>
   <si>
-    <t> /4500434590</t>
+    <t>/4500434590</t>
   </si>
   <si>
     <t>4700851680</t>
@@ -475,7 +492,7 @@
     <t>0491440900</t>
   </si>
   <si>
-    <t> /4500434694</t>
+    <t>/4500434694</t>
   </si>
   <si>
     <t>4700852017</t>
@@ -487,7 +504,7 @@
     <t>0491441081</t>
   </si>
   <si>
-    <t> /4500434963</t>
+    <t>/4500434963</t>
   </si>
   <si>
     <t>4700852428</t>
@@ -499,7 +516,7 @@
     <t>0491441415</t>
   </si>
   <si>
-    <t> /4500436295</t>
+    <t>/4500436295</t>
   </si>
   <si>
     <t>4700854993</t>
@@ -511,7 +528,7 @@
     <t>0491442690</t>
   </si>
   <si>
-    <t> /4500545113</t>
+    <t>/4500545113</t>
   </si>
   <si>
     <t>4700855231</t>
@@ -526,7 +543,7 @@
     <t>0491442890</t>
   </si>
   <si>
-    <t> /4500436879</t>
+    <t>/4500436879</t>
   </si>
   <si>
     <t>4700856339</t>
@@ -538,7 +555,7 @@
     <t>0491443451</t>
   </si>
   <si>
-    <t> /4500437317</t>
+    <t>/4500437317</t>
   </si>
   <si>
     <t>4700856657</t>
@@ -550,7 +567,7 @@
     <t>0491443586</t>
   </si>
   <si>
-    <t> /4500437324</t>
+    <t>/4500437324</t>
   </si>
   <si>
     <t>4700856868</t>
@@ -577,7 +594,7 @@
     <t>0491443883</t>
   </si>
   <si>
-    <t> /4500438011</t>
+    <t>/4500438011</t>
   </si>
   <si>
     <t>4700858479</t>
@@ -589,7 +606,7 @@
     <t>0491444466</t>
   </si>
   <si>
-    <t> /4500438064</t>
+    <t>/4500438064</t>
   </si>
   <si>
     <t>4700858756</t>
@@ -619,7 +636,7 @@
     <t>0491444729</t>
   </si>
   <si>
-    <t> /491418190</t>
+    <t>/491418190</t>
   </si>
   <si>
     <t>4810111828</t>
@@ -631,13 +648,13 @@
     <t>CCuervo Devolucion</t>
   </si>
   <si>
-    <t> /491430115</t>
+    <t>/491430115</t>
   </si>
   <si>
     <t>4810113981</t>
   </si>
   <si>
-    <t> /491442890</t>
+    <t>/491442890</t>
   </si>
   <si>
     <t>4810115676</t>
@@ -767,28 +784,67 @@
   </si>
   <si>
     <t>Gpo.Clientes</t>
+  </si>
+  <si>
+    <t>total_facturas</t>
+  </si>
+  <si>
+    <t>total_requis</t>
+  </si>
+  <si>
+    <t>orden_compra</t>
+  </si>
+  <si>
+    <t>confirmacion_cita</t>
+  </si>
+  <si>
+    <t>sua</t>
+  </si>
+  <si>
+    <t>certificados_sane</t>
+  </si>
+  <si>
+    <t>certificados_crt</t>
+  </si>
+  <si>
+    <t>lista_empaque</t>
+  </si>
+  <si>
+    <t>formato codigo_barras</t>
+  </si>
+  <si>
+    <t>bitacora_hoja_ingreso</t>
+  </si>
+  <si>
+    <t>bts_certificado_fumigacion</t>
+  </si>
+  <si>
+    <t>alarmas_aceptadas</t>
+  </si>
+  <si>
+    <t>ticket</t>
+  </si>
+  <si>
+    <t>comprobante_validacion_facturas</t>
+  </si>
+  <si>
+    <t>envio_template_pdf_xml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -798,18 +854,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,21 +882,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -865,77 +905,374 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AT59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BI59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AU1" sqref="AU1:BI1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="12" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="9" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="7" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="19" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="14" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="12" customWidth="1"/>
-    <col min="7" max="7" bestFit="1" width="12" customWidth="1"/>
-    <col min="8" max="8" bestFit="1" width="24" customWidth="1"/>
-    <col min="9" max="9" bestFit="1" width="20" customWidth="1"/>
-    <col min="10" max="10" bestFit="1" width="11" customWidth="1"/>
-    <col min="11" max="11" bestFit="1" width="17" customWidth="1"/>
-    <col min="12" max="12" bestFit="1" width="19" customWidth="1"/>
-    <col min="13" max="13" bestFit="1" width="13" customWidth="1"/>
-    <col min="14" max="14" bestFit="1" width="14" customWidth="1"/>
-    <col min="15" max="15" bestFit="1" width="13" customWidth="1"/>
-    <col min="16" max="16" bestFit="1" width="18" customWidth="1"/>
-    <col min="17" max="17" bestFit="1" width="10" customWidth="1"/>
-    <col min="18" max="18" bestFit="1" width="15" customWidth="1"/>
-    <col min="19" max="19" bestFit="1" width="13" customWidth="1"/>
-    <col min="20" max="20" bestFit="1" width="14" customWidth="1"/>
-    <col min="21" max="21" bestFit="1" width="15" customWidth="1"/>
-    <col min="22" max="22" bestFit="1" width="13" customWidth="1"/>
-    <col min="23" max="23" bestFit="1" width="13" customWidth="1"/>
-    <col min="24" max="24" bestFit="1" width="13" customWidth="1"/>
-    <col min="25" max="25" bestFit="1" width="9" customWidth="1"/>
-    <col min="26" max="26" bestFit="1" width="20" customWidth="1"/>
-    <col min="27" max="27" bestFit="1" width="5" customWidth="1"/>
-    <col min="28" max="28" bestFit="1" width="12" customWidth="1"/>
-    <col min="29" max="29" bestFit="1" width="12" customWidth="1"/>
-    <col min="30" max="30" bestFit="1" width="11" customWidth="1"/>
-    <col min="31" max="31" bestFit="1" width="10" customWidth="1"/>
-    <col min="32" max="32" bestFit="1" width="11" customWidth="1"/>
-    <col min="33" max="33" bestFit="1" width="6" customWidth="1"/>
-    <col min="34" max="34" bestFit="1" width="4" customWidth="1"/>
-    <col min="35" max="35" bestFit="1" width="19" customWidth="1"/>
-    <col min="36" max="36" bestFit="1" width="20" customWidth="1"/>
-    <col min="37" max="37" bestFit="1" width="40" customWidth="1"/>
-    <col min="38" max="38" bestFit="1" width="14" customWidth="1"/>
-    <col min="39" max="39" bestFit="1" width="12" customWidth="1"/>
-    <col min="40" max="40" bestFit="1" width="12" customWidth="1"/>
-    <col min="41" max="41" bestFit="1" width="16" customWidth="1"/>
-    <col min="42" max="42" bestFit="1" width="20" customWidth="1"/>
-    <col min="43" max="43" bestFit="1" width="12" customWidth="1"/>
-    <col min="44" max="44" bestFit="1" width="5" customWidth="1"/>
-    <col min="45" max="45" bestFit="1" width="14" customWidth="1"/>
-    <col min="46" max="46" bestFit="1" width="14" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="40" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="12" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="20" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="0" spans="">
+    <row r="1" spans="1:61" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>210</v>
       </c>
@@ -1074,8 +1411,53 @@
       <c r="AT1" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="AU1" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="AW1" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX1" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="AY1" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="AZ1" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="BA1" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="BB1" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="BC1" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="BD1" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="BE1" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="BF1" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="BH1" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="BI1" s="7" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="2" spans="1:46">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1101,34 +1483,34 @@
         <v>7</v>
       </c>
       <c r="I2" s="2">
-        <v>1576.000</v>
+        <v>1576</v>
       </c>
       <c r="J2" s="2">
-        <v>2101.333</v>
+        <v>2101.3330000000001</v>
       </c>
       <c r="K2" s="2">
-        <v>1576.000</v>
+        <v>1576</v>
       </c>
       <c r="L2" s="2">
-        <v>2101.333</v>
+        <v>2101.3330000000001</v>
       </c>
       <c r="M2" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N2" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>1576.000</v>
+        <v>1576</v>
       </c>
       <c r="P2" s="2">
-        <v>2101.333</v>
+        <v>2101.3330000000001</v>
       </c>
       <c r="Q2" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R2" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S2" s="4">
         <v>43444</v>
@@ -1211,7 +1593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:46">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1237,34 +1619,34 @@
         <v>7</v>
       </c>
       <c r="I3" s="2">
-        <v>26.000</v>
+        <v>26</v>
       </c>
       <c r="J3" s="2">
-        <v>30.333</v>
+        <v>30.332999999999998</v>
       </c>
       <c r="K3" s="2">
-        <v>26.000</v>
+        <v>26</v>
       </c>
       <c r="L3" s="2">
-        <v>30.333</v>
+        <v>30.332999999999998</v>
       </c>
       <c r="M3" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N3" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
-        <v>26.000</v>
+        <v>26</v>
       </c>
       <c r="P3" s="2">
-        <v>30.333</v>
+        <v>30.332999999999998</v>
       </c>
       <c r="Q3" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R3" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S3" s="4">
         <v>43444</v>
@@ -1347,7 +1729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:46">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1373,34 +1755,34 @@
         <v>7</v>
       </c>
       <c r="I4" s="2">
-        <v>402.000</v>
+        <v>402</v>
       </c>
       <c r="J4" s="2">
-        <v>536.000</v>
+        <v>536</v>
       </c>
       <c r="K4" s="2">
-        <v>402.000</v>
+        <v>402</v>
       </c>
       <c r="L4" s="2">
-        <v>536.000</v>
+        <v>536</v>
       </c>
       <c r="M4" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="2">
-        <v>402.000</v>
+        <v>402</v>
       </c>
       <c r="P4" s="2">
-        <v>536.000</v>
+        <v>536</v>
       </c>
       <c r="Q4" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="4">
         <v>43444</v>
@@ -1483,7 +1865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:46">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1509,34 +1891,34 @@
         <v>7</v>
       </c>
       <c r="I5" s="2">
-        <v>11121.000</v>
+        <v>11121</v>
       </c>
       <c r="J5" s="2">
-        <v>7414.000</v>
+        <v>7414</v>
       </c>
       <c r="K5" s="2">
-        <v>11121.000</v>
+        <v>11121</v>
       </c>
       <c r="L5" s="2">
-        <v>7414.000</v>
+        <v>7414</v>
       </c>
       <c r="M5" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N5" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O5" s="2">
-        <v>11121.000</v>
+        <v>11121</v>
       </c>
       <c r="P5" s="2">
-        <v>7414.000</v>
+        <v>7414</v>
       </c>
       <c r="Q5" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R5" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S5" s="4">
         <v>43446</v>
@@ -1592,7 +1974,7 @@
         <v>29</v>
       </c>
       <c r="AL5" s="5">
-        <v>2205405.51</v>
+        <v>2205405.5099999998</v>
       </c>
       <c r="AM5" t="s">
         <v>30</v>
@@ -1619,7 +2001,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:46">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1645,34 +2027,34 @@
         <v>7</v>
       </c>
       <c r="I6" s="2">
-        <v>15574.000</v>
+        <v>15574</v>
       </c>
       <c r="J6" s="2">
-        <v>20765.333</v>
+        <v>20765.332999999999</v>
       </c>
       <c r="K6" s="2">
-        <v>15574.000</v>
+        <v>15574</v>
       </c>
       <c r="L6" s="2">
-        <v>20765.333</v>
+        <v>20765.332999999999</v>
       </c>
       <c r="M6" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N6" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O6" s="2">
-        <v>15574.000</v>
+        <v>15574</v>
       </c>
       <c r="P6" s="2">
-        <v>20765.333</v>
+        <v>20765.332999999999</v>
       </c>
       <c r="Q6" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R6" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S6" s="4">
         <v>43452</v>
@@ -1755,7 +2137,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:46">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1781,34 +2163,34 @@
         <v>7</v>
       </c>
       <c r="I7" s="2">
-        <v>3388.000</v>
+        <v>3388</v>
       </c>
       <c r="J7" s="2">
-        <v>3952.667</v>
+        <v>3952.6669999999999</v>
       </c>
       <c r="K7" s="2">
-        <v>3388.000</v>
+        <v>3388</v>
       </c>
       <c r="L7" s="2">
-        <v>3952.667</v>
+        <v>3952.6669999999999</v>
       </c>
       <c r="M7" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O7" s="2">
-        <v>3388.000</v>
+        <v>3388</v>
       </c>
       <c r="P7" s="2">
-        <v>3952.667</v>
+        <v>3952.6669999999999</v>
       </c>
       <c r="Q7" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R7" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S7" s="4">
         <v>43462</v>
@@ -1891,7 +2273,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1917,34 +2299,34 @@
         <v>7</v>
       </c>
       <c r="I8" s="2">
-        <v>27752.000</v>
+        <v>27752</v>
       </c>
       <c r="J8" s="2">
-        <v>18501.333</v>
+        <v>18501.332999999999</v>
       </c>
       <c r="K8" s="2">
-        <v>9848.000</v>
+        <v>9848</v>
       </c>
       <c r="L8" s="2">
-        <v>6565.333</v>
+        <v>6565.3329999999996</v>
       </c>
       <c r="M8" s="2">
-        <v>17904.000</v>
+        <v>17904</v>
       </c>
       <c r="N8" s="2">
-        <v>11936.000</v>
+        <v>11936</v>
       </c>
       <c r="O8" s="2">
-        <v>2643.000</v>
+        <v>2643</v>
       </c>
       <c r="P8" s="2">
-        <v>1762.000</v>
+        <v>1762</v>
       </c>
       <c r="Q8" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R8" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S8" s="4">
         <v>43462</v>
@@ -2000,7 +2382,7 @@
         <v>29</v>
       </c>
       <c r="AL8" s="5">
-        <v>5503499.12</v>
+        <v>5503499.1200000001</v>
       </c>
       <c r="AM8" t="s">
         <v>42</v>
@@ -2027,7 +2409,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2053,34 +2435,34 @@
         <v>7</v>
       </c>
       <c r="I9" s="2">
-        <v>2000.000</v>
+        <v>2000</v>
       </c>
       <c r="J9" s="2">
-        <v>1333.333</v>
+        <v>1333.3330000000001</v>
       </c>
       <c r="K9" s="2">
-        <v>2000.000</v>
+        <v>2000</v>
       </c>
       <c r="L9" s="2">
-        <v>1333.333</v>
+        <v>1333.3330000000001</v>
       </c>
       <c r="M9" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O9" s="2">
-        <v>1260.000</v>
+        <v>1260</v>
       </c>
       <c r="P9" s="2">
-        <v>840.000</v>
+        <v>840</v>
       </c>
       <c r="Q9" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R9" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S9" s="4">
         <v>43462</v>
@@ -2136,7 +2518,7 @@
         <v>48</v>
       </c>
       <c r="AL9" s="5">
-        <v>389700.00</v>
+        <v>389700</v>
       </c>
       <c r="AM9" t="s">
         <v>49</v>
@@ -2163,7 +2545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2189,34 +2571,34 @@
         <v>7</v>
       </c>
       <c r="I10" s="2">
-        <v>3500.000</v>
+        <v>3500</v>
       </c>
       <c r="J10" s="2">
-        <v>4083.333</v>
+        <v>4083.3330000000001</v>
       </c>
       <c r="K10" s="2">
-        <v>3500.000</v>
+        <v>3500</v>
       </c>
       <c r="L10" s="2">
-        <v>4083.333</v>
+        <v>4083.3330000000001</v>
       </c>
       <c r="M10" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N10" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O10" s="2">
-        <v>512.000</v>
+        <v>512</v>
       </c>
       <c r="P10" s="2">
-        <v>597.333</v>
+        <v>597.33299999999997</v>
       </c>
       <c r="Q10" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R10" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S10" s="4">
         <v>43463</v>
@@ -2272,7 +2654,7 @@
         <v>22</v>
       </c>
       <c r="AL10" s="5">
-        <v>695310.00</v>
+        <v>695310</v>
       </c>
       <c r="AM10" t="s">
         <v>53</v>
@@ -2299,7 +2681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2325,34 +2707,34 @@
         <v>7</v>
       </c>
       <c r="I11" s="2">
-        <v>500.000</v>
+        <v>500</v>
       </c>
       <c r="J11" s="2">
-        <v>666.667</v>
+        <v>666.66700000000003</v>
       </c>
       <c r="K11" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="L11" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="M11" s="2">
-        <v>500.000</v>
+        <v>500</v>
       </c>
       <c r="N11" s="2">
-        <v>666.667</v>
+        <v>666.66700000000003</v>
       </c>
       <c r="O11" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="P11" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R11" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S11" s="4">
         <v>43463</v>
@@ -2404,7 +2786,7 @@
         <v>25</v>
       </c>
       <c r="AL11" s="5">
-        <v>104355.00</v>
+        <v>104355</v>
       </c>
       <c r="AM11" t="s">
         <v>14</v>
@@ -2431,7 +2813,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:46">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2457,34 +2839,34 @@
         <v>7</v>
       </c>
       <c r="I12" s="2">
-        <v>150.000</v>
+        <v>150</v>
       </c>
       <c r="J12" s="2">
-        <v>200.000</v>
+        <v>200</v>
       </c>
       <c r="K12" s="2">
-        <v>100.000</v>
+        <v>100</v>
       </c>
       <c r="L12" s="2">
         <v>133.333</v>
       </c>
       <c r="M12" s="2">
-        <v>50.000</v>
+        <v>50</v>
       </c>
       <c r="N12" s="2">
-        <v>66.667</v>
+        <v>66.667000000000002</v>
       </c>
       <c r="O12" s="2">
-        <v>100.000</v>
+        <v>100</v>
       </c>
       <c r="P12" s="2">
         <v>133.333</v>
       </c>
       <c r="Q12" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R12" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S12" s="4">
         <v>43464</v>
@@ -2540,7 +2922,7 @@
         <v>17</v>
       </c>
       <c r="AL12" s="5">
-        <v>29344.50</v>
+        <v>29344.5</v>
       </c>
       <c r="AM12" t="s">
         <v>57</v>
@@ -2567,7 +2949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:46">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2593,34 +2975,34 @@
         <v>7</v>
       </c>
       <c r="I13" s="2">
-        <v>10.000</v>
+        <v>10</v>
       </c>
       <c r="J13" s="2">
-        <v>16.000</v>
+        <v>16</v>
       </c>
       <c r="K13" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="L13" s="2">
-        <v>1.600</v>
+        <v>1.6</v>
       </c>
       <c r="M13" s="2">
-        <v>9.000</v>
+        <v>9</v>
       </c>
       <c r="N13" s="2">
-        <v>14.400</v>
+        <v>14.4</v>
       </c>
       <c r="O13" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
-        <v>1.600</v>
+        <v>1.6</v>
       </c>
       <c r="Q13" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R13" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S13" s="4">
         <v>43464</v>
@@ -2676,7 +3058,7 @@
         <v>60</v>
       </c>
       <c r="AL13" s="5">
-        <v>2806.30</v>
+        <v>2806.3</v>
       </c>
       <c r="AM13" t="s">
         <v>61</v>
@@ -2703,7 +3085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:46">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2729,34 +3111,34 @@
         <v>7</v>
       </c>
       <c r="I14" s="2">
-        <v>4200.000</v>
+        <v>4200</v>
       </c>
       <c r="J14" s="2">
-        <v>2800.000</v>
+        <v>2800</v>
       </c>
       <c r="K14" s="2">
-        <v>4200.000</v>
+        <v>4200</v>
       </c>
       <c r="L14" s="2">
-        <v>2800.000</v>
+        <v>2800</v>
       </c>
       <c r="M14" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N14" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>2099.000</v>
+        <v>2099</v>
       </c>
       <c r="P14" s="2">
-        <v>1399.333</v>
+        <v>1399.3330000000001</v>
       </c>
       <c r="Q14" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R14" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S14" s="4">
         <v>43479</v>
@@ -2812,7 +3194,7 @@
         <v>48</v>
       </c>
       <c r="AL14" s="5">
-        <v>900144.00</v>
+        <v>900144</v>
       </c>
       <c r="AM14" t="s">
         <v>65</v>
@@ -2839,7 +3221,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:46">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2865,34 +3247,34 @@
         <v>7</v>
       </c>
       <c r="I15" s="2">
-        <v>23451.000</v>
+        <v>23451</v>
       </c>
       <c r="J15" s="2">
-        <v>15634.000</v>
+        <v>15634</v>
       </c>
       <c r="K15" s="2">
-        <v>22901.000</v>
+        <v>22901</v>
       </c>
       <c r="L15" s="2">
-        <v>15267.333</v>
+        <v>15267.333000000001</v>
       </c>
       <c r="M15" s="2">
-        <v>550.000</v>
+        <v>550</v>
       </c>
       <c r="N15" s="2">
-        <v>366.667</v>
+        <v>366.66699999999997</v>
       </c>
       <c r="O15" s="2">
-        <v>22851.000</v>
+        <v>22851</v>
       </c>
       <c r="P15" s="2">
-        <v>15234.000</v>
+        <v>15234</v>
       </c>
       <c r="Q15" s="2">
-        <v>50.000</v>
+        <v>50</v>
       </c>
       <c r="R15" s="2">
-        <v>33.333</v>
+        <v>33.332999999999998</v>
       </c>
       <c r="S15" s="4">
         <v>43482</v>
@@ -2975,7 +3357,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:46">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -3001,34 +3383,34 @@
         <v>7</v>
       </c>
       <c r="I16" s="2">
-        <v>17000.000</v>
+        <v>17000</v>
       </c>
       <c r="J16" s="2">
-        <v>22666.667</v>
+        <v>22666.667000000001</v>
       </c>
       <c r="K16" s="2">
-        <v>16314.000</v>
+        <v>16314</v>
       </c>
       <c r="L16" s="2">
-        <v>21752.000</v>
+        <v>21752</v>
       </c>
       <c r="M16" s="2">
-        <v>686.000</v>
+        <v>686</v>
       </c>
       <c r="N16" s="2">
-        <v>914.667</v>
+        <v>914.66700000000003</v>
       </c>
       <c r="O16" s="2">
-        <v>16314.000</v>
+        <v>16314</v>
       </c>
       <c r="P16" s="2">
-        <v>21752.000</v>
+        <v>21752</v>
       </c>
       <c r="Q16" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R16" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S16" s="4">
         <v>43510</v>
@@ -3084,7 +3466,7 @@
         <v>17</v>
       </c>
       <c r="AL16" s="5">
-        <v>3571190.00</v>
+        <v>3571190</v>
       </c>
       <c r="AM16" t="s">
         <v>74</v>
@@ -3111,7 +3493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:46">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -3137,34 +3519,34 @@
         <v>7</v>
       </c>
       <c r="I17" s="2">
-        <v>5000.000</v>
+        <v>5000</v>
       </c>
       <c r="J17" s="2">
-        <v>8000.000</v>
+        <v>8000</v>
       </c>
       <c r="K17" s="2">
-        <v>5000.000</v>
+        <v>5000</v>
       </c>
       <c r="L17" s="2">
-        <v>8000.000</v>
+        <v>8000</v>
       </c>
       <c r="M17" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N17" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O17" s="2">
-        <v>5000.000</v>
+        <v>5000</v>
       </c>
       <c r="P17" s="2">
-        <v>8000.000</v>
+        <v>8000</v>
       </c>
       <c r="Q17" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R17" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S17" s="4">
         <v>43510</v>
@@ -3220,7 +3602,7 @@
         <v>60</v>
       </c>
       <c r="AL17" s="5">
-        <v>1486450.00</v>
+        <v>1486450</v>
       </c>
       <c r="AM17" t="s">
         <v>76</v>
@@ -3247,7 +3629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:46">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -3273,34 +3655,34 @@
         <v>7</v>
       </c>
       <c r="I18" s="2">
-        <v>3761.000</v>
+        <v>3761</v>
       </c>
       <c r="J18" s="2">
-        <v>5014.667</v>
+        <v>5014.6670000000004</v>
       </c>
       <c r="K18" s="2">
-        <v>3761.000</v>
+        <v>3761</v>
       </c>
       <c r="L18" s="2">
-        <v>5014.667</v>
+        <v>5014.6670000000004</v>
       </c>
       <c r="M18" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N18" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>3761.000</v>
+        <v>3761</v>
       </c>
       <c r="P18" s="2">
-        <v>5014.667</v>
+        <v>5014.6670000000004</v>
       </c>
       <c r="Q18" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R18" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S18" s="4">
         <v>43510</v>
@@ -3383,7 +3765,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:46">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -3409,34 +3791,34 @@
         <v>7</v>
       </c>
       <c r="I19" s="2">
-        <v>6586.000</v>
+        <v>6586</v>
       </c>
       <c r="J19" s="2">
-        <v>7683.667</v>
+        <v>7683.6670000000004</v>
       </c>
       <c r="K19" s="2">
-        <v>6586.000</v>
+        <v>6586</v>
       </c>
       <c r="L19" s="2">
-        <v>7683.667</v>
+        <v>7683.6670000000004</v>
       </c>
       <c r="M19" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N19" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O19" s="2">
-        <v>6586.000</v>
+        <v>6586</v>
       </c>
       <c r="P19" s="2">
-        <v>7683.667</v>
+        <v>7683.6670000000004</v>
       </c>
       <c r="Q19" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R19" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S19" s="4">
         <v>43523</v>
@@ -3519,7 +3901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:46">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -3545,34 +3927,34 @@
         <v>7</v>
       </c>
       <c r="I20" s="2">
-        <v>1734.000</v>
+        <v>1734</v>
       </c>
       <c r="J20" s="2">
-        <v>1156.000</v>
+        <v>1156</v>
       </c>
       <c r="K20" s="2">
-        <v>1733.000</v>
+        <v>1733</v>
       </c>
       <c r="L20" s="2">
-        <v>1155.333</v>
+        <v>1155.3330000000001</v>
       </c>
       <c r="M20" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="N20" s="2">
-        <v>0.667</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="O20" s="2">
-        <v>1733.000</v>
+        <v>1733</v>
       </c>
       <c r="P20" s="2">
-        <v>1155.333</v>
+        <v>1155.3330000000001</v>
       </c>
       <c r="Q20" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R20" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S20" s="4">
         <v>43523</v>
@@ -3655,7 +4037,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:46">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -3681,34 +4063,34 @@
         <v>7</v>
       </c>
       <c r="I21" s="2">
-        <v>15094.000</v>
+        <v>15094</v>
       </c>
       <c r="J21" s="2">
-        <v>20125.333</v>
+        <v>20125.332999999999</v>
       </c>
       <c r="K21" s="2">
-        <v>15094.000</v>
+        <v>15094</v>
       </c>
       <c r="L21" s="2">
-        <v>20125.333</v>
+        <v>20125.332999999999</v>
       </c>
       <c r="M21" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N21" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O21" s="2">
-        <v>15094.000</v>
+        <v>15094</v>
       </c>
       <c r="P21" s="2">
-        <v>20125.333</v>
+        <v>20125.332999999999</v>
       </c>
       <c r="Q21" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R21" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S21" s="4">
         <v>43543</v>
@@ -3791,7 +4173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:46">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -3817,34 +4199,34 @@
         <v>7</v>
       </c>
       <c r="I22" s="2">
-        <v>3076.000</v>
+        <v>3076</v>
       </c>
       <c r="J22" s="2">
-        <v>4921.600</v>
+        <v>4921.6000000000004</v>
       </c>
       <c r="K22" s="2">
-        <v>3076.000</v>
+        <v>3076</v>
       </c>
       <c r="L22" s="2">
-        <v>4921.600</v>
+        <v>4921.6000000000004</v>
       </c>
       <c r="M22" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N22" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O22" s="2">
-        <v>3076.000</v>
+        <v>3076</v>
       </c>
       <c r="P22" s="2">
-        <v>4921.600</v>
+        <v>4921.6000000000004</v>
       </c>
       <c r="Q22" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R22" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S22" s="4">
         <v>43543</v>
@@ -3927,7 +4309,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:46">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -3953,34 +4335,34 @@
         <v>7</v>
       </c>
       <c r="I23" s="2">
-        <v>3169.000</v>
+        <v>3169</v>
       </c>
       <c r="J23" s="2">
-        <v>4225.333</v>
+        <v>4225.3329999999996</v>
       </c>
       <c r="K23" s="2">
-        <v>3169.000</v>
+        <v>3169</v>
       </c>
       <c r="L23" s="2">
-        <v>4225.333</v>
+        <v>4225.3329999999996</v>
       </c>
       <c r="M23" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N23" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O23" s="2">
-        <v>3169.000</v>
+        <v>3169</v>
       </c>
       <c r="P23" s="2">
-        <v>4225.333</v>
+        <v>4225.3329999999996</v>
       </c>
       <c r="Q23" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R23" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S23" s="4">
         <v>43543</v>
@@ -4063,7 +4445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:46">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -4089,34 +4471,34 @@
         <v>7</v>
       </c>
       <c r="I24" s="2">
-        <v>1300.000</v>
+        <v>1300</v>
       </c>
       <c r="J24" s="2">
-        <v>2080.000</v>
+        <v>2080</v>
       </c>
       <c r="K24" s="2">
-        <v>82.000</v>
+        <v>82</v>
       </c>
       <c r="L24" s="2">
-        <v>131.200</v>
+        <v>131.19999999999999</v>
       </c>
       <c r="M24" s="2">
-        <v>1218.000</v>
+        <v>1218</v>
       </c>
       <c r="N24" s="2">
-        <v>1948.800</v>
+        <v>1948.8</v>
       </c>
       <c r="O24" s="2">
-        <v>82.000</v>
+        <v>82</v>
       </c>
       <c r="P24" s="2">
-        <v>131.200</v>
+        <v>131.19999999999999</v>
       </c>
       <c r="Q24" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R24" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S24" s="4">
         <v>43584</v>
@@ -4172,7 +4554,7 @@
         <v>60</v>
       </c>
       <c r="AL24" s="5">
-        <v>386477.00</v>
+        <v>386477</v>
       </c>
       <c r="AM24" t="s">
         <v>90</v>
@@ -4199,7 +4581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:46">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -4225,34 +4607,34 @@
         <v>7</v>
       </c>
       <c r="I25" s="2">
-        <v>2255.000</v>
+        <v>2255</v>
       </c>
       <c r="J25" s="2">
-        <v>1503.333</v>
+        <v>1503.3330000000001</v>
       </c>
       <c r="K25" s="2">
-        <v>1835.000</v>
+        <v>1835</v>
       </c>
       <c r="L25" s="2">
-        <v>1223.333</v>
+        <v>1223.3330000000001</v>
       </c>
       <c r="M25" s="2">
-        <v>420.000</v>
+        <v>420</v>
       </c>
       <c r="N25" s="2">
-        <v>280.000</v>
+        <v>280</v>
       </c>
       <c r="O25" s="2">
-        <v>1835.000</v>
+        <v>1835</v>
       </c>
       <c r="P25" s="2">
-        <v>1223.333</v>
+        <v>1223.3330000000001</v>
       </c>
       <c r="Q25" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R25" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S25" s="4">
         <v>43584</v>
@@ -4308,7 +4690,7 @@
         <v>48</v>
       </c>
       <c r="AL25" s="5">
-        <v>483291.60</v>
+        <v>483291.6</v>
       </c>
       <c r="AM25" t="s">
         <v>90</v>
@@ -4335,7 +4717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:46">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -4361,34 +4743,34 @@
         <v>7</v>
       </c>
       <c r="I26" s="2">
-        <v>7904.000</v>
+        <v>7904</v>
       </c>
       <c r="J26" s="2">
-        <v>9221.333</v>
+        <v>9221.3330000000005</v>
       </c>
       <c r="K26" s="2">
-        <v>7898.000</v>
+        <v>7898</v>
       </c>
       <c r="L26" s="2">
-        <v>9214.333</v>
+        <v>9214.3330000000005</v>
       </c>
       <c r="M26" s="2">
-        <v>6.000</v>
+        <v>6</v>
       </c>
       <c r="N26" s="2">
-        <v>7.000</v>
+        <v>7</v>
       </c>
       <c r="O26" s="2">
-        <v>7898.000</v>
+        <v>7898</v>
       </c>
       <c r="P26" s="2">
-        <v>9214.333</v>
+        <v>9214.3330000000005</v>
       </c>
       <c r="Q26" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R26" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S26" s="4">
         <v>43584</v>
@@ -4471,7 +4853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:46">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -4497,34 +4879,34 @@
         <v>7</v>
       </c>
       <c r="I27" s="2">
-        <v>12015.000</v>
+        <v>12015</v>
       </c>
       <c r="J27" s="2">
-        <v>16020.000</v>
+        <v>16020</v>
       </c>
       <c r="K27" s="2">
-        <v>12015.000</v>
+        <v>12015</v>
       </c>
       <c r="L27" s="2">
-        <v>16020.000</v>
+        <v>16020</v>
       </c>
       <c r="M27" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N27" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O27" s="2">
-        <v>12015.000</v>
+        <v>12015</v>
       </c>
       <c r="P27" s="2">
-        <v>16020.000</v>
+        <v>16020</v>
       </c>
       <c r="Q27" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R27" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S27" s="4">
         <v>43584</v>
@@ -4580,7 +4962,7 @@
         <v>94</v>
       </c>
       <c r="AL27" s="5">
-        <v>2523991.05</v>
+        <v>2523991.0499999998</v>
       </c>
       <c r="AM27" t="s">
         <v>90</v>
@@ -4607,7 +4989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:46">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -4633,34 +5015,34 @@
         <v>7</v>
       </c>
       <c r="I28" s="2">
-        <v>2500.000</v>
+        <v>2500</v>
       </c>
       <c r="J28" s="2">
-        <v>3333.333</v>
+        <v>3333.3330000000001</v>
       </c>
       <c r="K28" s="2">
-        <v>2500.000</v>
+        <v>2500</v>
       </c>
       <c r="L28" s="2">
-        <v>3333.333</v>
+        <v>3333.3330000000001</v>
       </c>
       <c r="M28" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N28" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O28" s="2">
-        <v>2438.000</v>
+        <v>2438</v>
       </c>
       <c r="P28" s="2">
-        <v>3250.667</v>
+        <v>3250.6669999999999</v>
       </c>
       <c r="Q28" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R28" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S28" s="4">
         <v>43584</v>
@@ -4716,7 +5098,7 @@
         <v>97</v>
       </c>
       <c r="AL28" s="5">
-        <v>555075.00</v>
+        <v>555075</v>
       </c>
       <c r="AM28" t="s">
         <v>90</v>
@@ -4743,7 +5125,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:46">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -4769,34 +5151,34 @@
         <v>7</v>
       </c>
       <c r="I29" s="2">
-        <v>2923.000</v>
+        <v>2923</v>
       </c>
       <c r="J29" s="2">
-        <v>3410.167</v>
+        <v>3410.1669999999999</v>
       </c>
       <c r="K29" s="2">
-        <v>2923.000</v>
+        <v>2923</v>
       </c>
       <c r="L29" s="2">
-        <v>3410.167</v>
+        <v>3410.1669999999999</v>
       </c>
       <c r="M29" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N29" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O29" s="2">
-        <v>2923.000</v>
+        <v>2923</v>
       </c>
       <c r="P29" s="2">
-        <v>3410.167</v>
+        <v>3410.1669999999999</v>
       </c>
       <c r="Q29" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R29" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S29" s="4">
         <v>43605</v>
@@ -4879,7 +5261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:46">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -4905,34 +5287,34 @@
         <v>7</v>
       </c>
       <c r="I30" s="2">
-        <v>31886.000</v>
+        <v>31886</v>
       </c>
       <c r="J30" s="2">
-        <v>42514.667</v>
+        <v>42514.667000000001</v>
       </c>
       <c r="K30" s="2">
-        <v>31886.000</v>
+        <v>31886</v>
       </c>
       <c r="L30" s="2">
-        <v>42514.667</v>
+        <v>42514.667000000001</v>
       </c>
       <c r="M30" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N30" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O30" s="2">
-        <v>6804.000</v>
+        <v>6804</v>
       </c>
       <c r="P30" s="2">
-        <v>9072.000</v>
+        <v>9072</v>
       </c>
       <c r="Q30" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R30" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S30" s="4">
         <v>43606</v>
@@ -4988,7 +5370,7 @@
         <v>94</v>
       </c>
       <c r="AL30" s="5">
-        <v>6698292.02</v>
+        <v>6698292.0199999996</v>
       </c>
       <c r="AM30" t="s">
         <v>106</v>
@@ -5015,7 +5397,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:46">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -5041,34 +5423,34 @@
         <v>7</v>
       </c>
       <c r="I31" s="2">
-        <v>130.000</v>
+        <v>130</v>
       </c>
       <c r="J31" s="2">
         <v>151.667</v>
       </c>
       <c r="K31" s="2">
-        <v>123.000</v>
+        <v>123</v>
       </c>
       <c r="L31" s="2">
-        <v>143.500</v>
+        <v>143.5</v>
       </c>
       <c r="M31" s="2">
-        <v>7.000</v>
+        <v>7</v>
       </c>
       <c r="N31" s="2">
-        <v>8.167</v>
+        <v>8.1669999999999998</v>
       </c>
       <c r="O31" s="2">
-        <v>123.000</v>
+        <v>123</v>
       </c>
       <c r="P31" s="2">
-        <v>143.500</v>
+        <v>143.5</v>
       </c>
       <c r="Q31" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R31" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S31" s="4">
         <v>43607</v>
@@ -5124,7 +5506,7 @@
         <v>22</v>
       </c>
       <c r="AL31" s="5">
-        <v>27372.80</v>
+        <v>27372.799999999999</v>
       </c>
       <c r="AM31" t="s">
         <v>110</v>
@@ -5151,7 +5533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:46">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -5177,34 +5559,34 @@
         <v>7</v>
       </c>
       <c r="I32" s="2">
-        <v>4100.000</v>
+        <v>4100</v>
       </c>
       <c r="J32" s="2">
-        <v>4783.333</v>
+        <v>4783.3329999999996</v>
       </c>
       <c r="K32" s="2">
-        <v>4100.000</v>
+        <v>4100</v>
       </c>
       <c r="L32" s="2">
-        <v>4783.333</v>
+        <v>4783.3329999999996</v>
       </c>
       <c r="M32" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N32" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O32" s="2">
-        <v>3372.000</v>
+        <v>3372</v>
       </c>
       <c r="P32" s="2">
-        <v>3934.000</v>
+        <v>3934</v>
       </c>
       <c r="Q32" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R32" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S32" s="4">
         <v>43622</v>
@@ -5260,7 +5642,7 @@
         <v>101</v>
       </c>
       <c r="AL32" s="5">
-        <v>863296.00</v>
+        <v>863296</v>
       </c>
       <c r="AM32" t="s">
         <v>114</v>
@@ -5287,7 +5669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:46">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -5313,34 +5695,34 @@
         <v>7</v>
       </c>
       <c r="I33" s="2">
-        <v>9796.000</v>
+        <v>9796</v>
       </c>
       <c r="J33" s="2">
-        <v>6530.667</v>
+        <v>6530.6670000000004</v>
       </c>
       <c r="K33" s="2">
-        <v>9600.000</v>
+        <v>9600</v>
       </c>
       <c r="L33" s="2">
-        <v>6400.000</v>
+        <v>6400</v>
       </c>
       <c r="M33" s="2">
-        <v>196.000</v>
+        <v>196</v>
       </c>
       <c r="N33" s="2">
         <v>130.667</v>
       </c>
       <c r="O33" s="2">
-        <v>5114.000</v>
+        <v>5114</v>
       </c>
       <c r="P33" s="2">
-        <v>3409.333</v>
+        <v>3409.3330000000001</v>
       </c>
       <c r="Q33" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R33" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S33" s="4">
         <v>43641</v>
@@ -5423,7 +5805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:46">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -5449,34 +5831,34 @@
         <v>7</v>
       </c>
       <c r="I34" s="2">
-        <v>2147.000</v>
+        <v>2147</v>
       </c>
       <c r="J34" s="2">
-        <v>2862.667</v>
+        <v>2862.6669999999999</v>
       </c>
       <c r="K34" s="2">
-        <v>2147.000</v>
+        <v>2147</v>
       </c>
       <c r="L34" s="2">
-        <v>2862.667</v>
+        <v>2862.6669999999999</v>
       </c>
       <c r="M34" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N34" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O34" s="2">
-        <v>1979.000</v>
+        <v>1979</v>
       </c>
       <c r="P34" s="2">
-        <v>2638.667</v>
+        <v>2638.6669999999999</v>
       </c>
       <c r="Q34" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R34" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S34" s="4">
         <v>43641</v>
@@ -5559,7 +5941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:46">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -5585,34 +5967,34 @@
         <v>7</v>
       </c>
       <c r="I35" s="2">
-        <v>2624.000</v>
+        <v>2624</v>
       </c>
       <c r="J35" s="2">
-        <v>3498.667</v>
+        <v>3498.6669999999999</v>
       </c>
       <c r="K35" s="2">
-        <v>2562.000</v>
+        <v>2562</v>
       </c>
       <c r="L35" s="2">
-        <v>3416.000</v>
+        <v>3416</v>
       </c>
       <c r="M35" s="2">
-        <v>62.000</v>
+        <v>62</v>
       </c>
       <c r="N35" s="2">
-        <v>82.667</v>
+        <v>82.667000000000002</v>
       </c>
       <c r="O35" s="2">
-        <v>2562.000</v>
+        <v>2562</v>
       </c>
       <c r="P35" s="2">
-        <v>3416.000</v>
+        <v>3416</v>
       </c>
       <c r="Q35" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R35" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S35" s="4">
         <v>43641</v>
@@ -5695,7 +6077,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:46">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -5721,34 +6103,34 @@
         <v>7</v>
       </c>
       <c r="I36" s="2">
-        <v>6500.000</v>
+        <v>6500</v>
       </c>
       <c r="J36" s="2">
-        <v>4333.333</v>
+        <v>4333.3329999999996</v>
       </c>
       <c r="K36" s="2">
-        <v>6500.000</v>
+        <v>6500</v>
       </c>
       <c r="L36" s="2">
-        <v>4333.333</v>
+        <v>4333.3329999999996</v>
       </c>
       <c r="M36" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N36" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O36" s="2">
-        <v>3043.000</v>
+        <v>3043</v>
       </c>
       <c r="P36" s="2">
-        <v>2028.667</v>
+        <v>2028.6669999999999</v>
       </c>
       <c r="Q36" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R36" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S36" s="4">
         <v>43642</v>
@@ -5804,7 +6186,7 @@
         <v>129</v>
       </c>
       <c r="AL36" s="5">
-        <v>1393080.00</v>
+        <v>1393080</v>
       </c>
       <c r="AM36" t="s">
         <v>130</v>
@@ -5831,7 +6213,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:46">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -5857,34 +6239,34 @@
         <v>7</v>
       </c>
       <c r="I37" s="2">
-        <v>2982.000</v>
+        <v>2982</v>
       </c>
       <c r="J37" s="2">
-        <v>3976.000</v>
+        <v>3976</v>
       </c>
       <c r="K37" s="2">
-        <v>2982.000</v>
+        <v>2982</v>
       </c>
       <c r="L37" s="2">
-        <v>3976.000</v>
+        <v>3976</v>
       </c>
       <c r="M37" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N37" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O37" s="2">
-        <v>2520.000</v>
+        <v>2520</v>
       </c>
       <c r="P37" s="2">
-        <v>3360.000</v>
+        <v>3360</v>
       </c>
       <c r="Q37" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R37" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S37" s="4">
         <v>43654</v>
@@ -5967,7 +6349,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:46">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -5993,34 +6375,34 @@
         <v>7</v>
       </c>
       <c r="I38" s="2">
-        <v>1525.000</v>
+        <v>1525</v>
       </c>
       <c r="J38" s="2">
-        <v>1779.167</v>
+        <v>1779.1669999999999</v>
       </c>
       <c r="K38" s="2">
-        <v>1525.000</v>
+        <v>1525</v>
       </c>
       <c r="L38" s="2">
-        <v>1779.167</v>
+        <v>1779.1669999999999</v>
       </c>
       <c r="M38" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N38" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O38" s="2">
-        <v>1525.000</v>
+        <v>1525</v>
       </c>
       <c r="P38" s="2">
-        <v>1779.167</v>
+        <v>1779.1669999999999</v>
       </c>
       <c r="Q38" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R38" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S38" s="4">
         <v>43654</v>
@@ -6076,7 +6458,7 @@
         <v>101</v>
       </c>
       <c r="AL38" s="5">
-        <v>321104.00</v>
+        <v>321104</v>
       </c>
       <c r="AM38" t="s">
         <v>136</v>
@@ -6103,7 +6485,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:46">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -6129,34 +6511,34 @@
         <v>7</v>
       </c>
       <c r="I39" s="2">
-        <v>234.000</v>
+        <v>234</v>
       </c>
       <c r="J39" s="2">
-        <v>273.000</v>
+        <v>273</v>
       </c>
       <c r="K39" s="2">
-        <v>234.000</v>
+        <v>234</v>
       </c>
       <c r="L39" s="2">
-        <v>273.000</v>
+        <v>273</v>
       </c>
       <c r="M39" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N39" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O39" s="2">
-        <v>234.000</v>
+        <v>234</v>
       </c>
       <c r="P39" s="2">
-        <v>273.000</v>
+        <v>273</v>
       </c>
       <c r="Q39" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R39" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S39" s="4">
         <v>43655</v>
@@ -6212,7 +6594,7 @@
         <v>101</v>
       </c>
       <c r="AL39" s="5">
-        <v>49271.04</v>
+        <v>49271.040000000001</v>
       </c>
       <c r="AM39" t="s">
         <v>140</v>
@@ -6239,7 +6621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:46">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -6265,34 +6647,34 @@
         <v>7</v>
       </c>
       <c r="I40" s="2">
-        <v>17048.000</v>
+        <v>17048</v>
       </c>
       <c r="J40" s="2">
-        <v>22730.667</v>
+        <v>22730.667000000001</v>
       </c>
       <c r="K40" s="2">
-        <v>17048.000</v>
+        <v>17048</v>
       </c>
       <c r="L40" s="2">
-        <v>22730.667</v>
+        <v>22730.667000000001</v>
       </c>
       <c r="M40" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N40" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O40" s="2">
-        <v>11928.000</v>
+        <v>11928</v>
       </c>
       <c r="P40" s="2">
-        <v>15904.000</v>
+        <v>15904</v>
       </c>
       <c r="Q40" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R40" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S40" s="4">
         <v>43656</v>
@@ -6375,7 +6757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:46">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -6401,34 +6783,34 @@
         <v>7</v>
       </c>
       <c r="I41" s="2">
-        <v>9787.000</v>
+        <v>9787</v>
       </c>
       <c r="J41" s="2">
-        <v>6524.667</v>
+        <v>6524.6670000000004</v>
       </c>
       <c r="K41" s="2">
-        <v>9139.000</v>
+        <v>9139</v>
       </c>
       <c r="L41" s="2">
-        <v>6092.667</v>
+        <v>6092.6670000000004</v>
       </c>
       <c r="M41" s="2">
-        <v>648.000</v>
+        <v>648</v>
       </c>
       <c r="N41" s="2">
-        <v>432.000</v>
+        <v>432</v>
       </c>
       <c r="O41" s="2">
-        <v>3604.000</v>
+        <v>3604</v>
       </c>
       <c r="P41" s="2">
-        <v>2402.667</v>
+        <v>2402.6669999999999</v>
       </c>
       <c r="Q41" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R41" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S41" s="4">
         <v>43656</v>
@@ -6511,7 +6893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:46">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -6537,34 +6919,34 @@
         <v>7</v>
       </c>
       <c r="I42" s="2">
-        <v>24980.000</v>
+        <v>24980</v>
       </c>
       <c r="J42" s="2">
-        <v>33306.667</v>
+        <v>33306.667000000001</v>
       </c>
       <c r="K42" s="2">
-        <v>24812.000</v>
+        <v>24812</v>
       </c>
       <c r="L42" s="2">
-        <v>33082.667</v>
+        <v>33082.667000000001</v>
       </c>
       <c r="M42" s="2">
-        <v>168.000</v>
+        <v>168</v>
       </c>
       <c r="N42" s="2">
-        <v>224.000</v>
+        <v>224</v>
       </c>
       <c r="O42" s="2">
-        <v>23426.000</v>
+        <v>23426</v>
       </c>
       <c r="P42" s="2">
-        <v>31234.667</v>
+        <v>31234.667000000001</v>
       </c>
       <c r="Q42" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R42" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S42" s="4">
         <v>43669</v>
@@ -6620,7 +7002,7 @@
         <v>94</v>
       </c>
       <c r="AL42" s="5">
-        <v>5247548.60</v>
+        <v>5247548.5999999996</v>
       </c>
       <c r="AM42" t="s">
         <v>152</v>
@@ -6647,7 +7029,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:46">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -6673,34 +7055,34 @@
         <v>7</v>
       </c>
       <c r="I43" s="2">
-        <v>1574.000</v>
+        <v>1574</v>
       </c>
       <c r="J43" s="2">
-        <v>2098.667</v>
+        <v>2098.6669999999999</v>
       </c>
       <c r="K43" s="2">
-        <v>1574.000</v>
+        <v>1574</v>
       </c>
       <c r="L43" s="2">
-        <v>2098.667</v>
+        <v>2098.6669999999999</v>
       </c>
       <c r="M43" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N43" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O43" s="2">
-        <v>1574.000</v>
+        <v>1574</v>
       </c>
       <c r="P43" s="2">
-        <v>2098.667</v>
+        <v>2098.6669999999999</v>
       </c>
       <c r="Q43" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R43" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S43" s="4">
         <v>43669</v>
@@ -6783,7 +7165,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:46">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -6809,34 +7191,34 @@
         <v>7</v>
       </c>
       <c r="I44" s="2">
-        <v>2535.000</v>
+        <v>2535</v>
       </c>
       <c r="J44" s="2">
-        <v>2957.500</v>
+        <v>2957.5</v>
       </c>
       <c r="K44" s="2">
-        <v>2535.000</v>
+        <v>2535</v>
       </c>
       <c r="L44" s="2">
-        <v>2957.500</v>
+        <v>2957.5</v>
       </c>
       <c r="M44" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N44" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O44" s="2">
-        <v>2262.000</v>
+        <v>2262</v>
       </c>
       <c r="P44" s="2">
-        <v>2639.000</v>
+        <v>2639</v>
       </c>
       <c r="Q44" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R44" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S44" s="4">
         <v>43671</v>
@@ -6892,7 +7274,7 @@
         <v>101</v>
       </c>
       <c r="AL44" s="5">
-        <v>533769.60</v>
+        <v>533769.6</v>
       </c>
       <c r="AM44" t="s">
         <v>156</v>
@@ -6919,7 +7301,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:46">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -6945,34 +7327,34 @@
         <v>7</v>
       </c>
       <c r="I45" s="2">
-        <v>3179.000</v>
+        <v>3179</v>
       </c>
       <c r="J45" s="2">
-        <v>3708.833</v>
+        <v>3708.8330000000001</v>
       </c>
       <c r="K45" s="2">
-        <v>3179.000</v>
+        <v>3179</v>
       </c>
       <c r="L45" s="2">
-        <v>3708.833</v>
+        <v>3708.8330000000001</v>
       </c>
       <c r="M45" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N45" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O45" s="2">
-        <v>3179.000</v>
+        <v>3179</v>
       </c>
       <c r="P45" s="2">
-        <v>3708.833</v>
+        <v>3708.8330000000001</v>
       </c>
       <c r="Q45" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R45" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S45" s="4">
         <v>43675</v>
@@ -7055,7 +7437,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:46">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -7081,34 +7463,34 @@
         <v>7</v>
       </c>
       <c r="I46" s="2">
-        <v>3021.000</v>
+        <v>3021</v>
       </c>
       <c r="J46" s="2">
-        <v>4028.000</v>
+        <v>4028</v>
       </c>
       <c r="K46" s="2">
-        <v>3021.000</v>
+        <v>3021</v>
       </c>
       <c r="L46" s="2">
-        <v>4028.000</v>
+        <v>4028</v>
       </c>
       <c r="M46" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N46" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O46" s="2">
-        <v>3021.000</v>
+        <v>3021</v>
       </c>
       <c r="P46" s="2">
-        <v>4028.000</v>
+        <v>4028</v>
       </c>
       <c r="Q46" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R46" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S46" s="4">
         <v>43692</v>
@@ -7191,7 +7573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:46">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -7217,34 +7599,34 @@
         <v>7</v>
       </c>
       <c r="I47" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="J47" s="2">
-        <v>0.667</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="K47" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="L47" s="2">
-        <v>0.667</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="M47" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N47" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O47" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="P47" s="2">
-        <v>0.667</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="Q47" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="R47" s="2">
-        <v>0.667</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="S47" s="4">
         <v>43695</v>
@@ -7331,7 +7713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:46">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -7357,34 +7739,34 @@
         <v>7</v>
       </c>
       <c r="I48" s="2">
-        <v>5499.000</v>
+        <v>5499</v>
       </c>
       <c r="J48" s="2">
-        <v>3666.000</v>
+        <v>3666</v>
       </c>
       <c r="K48" s="2">
-        <v>4749.000</v>
+        <v>4749</v>
       </c>
       <c r="L48" s="2">
-        <v>3166.000</v>
+        <v>3166</v>
       </c>
       <c r="M48" s="2">
-        <v>750.000</v>
+        <v>750</v>
       </c>
       <c r="N48" s="2">
-        <v>500.000</v>
+        <v>500</v>
       </c>
       <c r="O48" s="2">
-        <v>1935.000</v>
+        <v>1935</v>
       </c>
       <c r="P48" s="2">
-        <v>1290.000</v>
+        <v>1290</v>
       </c>
       <c r="Q48" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R48" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S48" s="4">
         <v>43703</v>
@@ -7442,7 +7824,7 @@
         <v>29</v>
       </c>
       <c r="AL48" s="5">
-        <v>1166447.88</v>
+        <v>1166447.8799999999</v>
       </c>
       <c r="AM48" t="s">
         <v>173</v>
@@ -7469,7 +7851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:46">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -7495,34 +7877,34 @@
         <v>7</v>
       </c>
       <c r="I49" s="2">
-        <v>1100.000</v>
+        <v>1100</v>
       </c>
       <c r="J49" s="2">
-        <v>1283.333</v>
+        <v>1283.3330000000001</v>
       </c>
       <c r="K49" s="2">
-        <v>1100.000</v>
+        <v>1100</v>
       </c>
       <c r="L49" s="2">
-        <v>1283.333</v>
+        <v>1283.3330000000001</v>
       </c>
       <c r="M49" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N49" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O49" s="2">
-        <v>1100.000</v>
+        <v>1100</v>
       </c>
       <c r="P49" s="2">
-        <v>1283.333</v>
+        <v>1283.3330000000001</v>
       </c>
       <c r="Q49" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R49" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S49" s="4">
         <v>43704</v>
@@ -7580,7 +7962,7 @@
         <v>101</v>
       </c>
       <c r="AL49" s="5">
-        <v>231616.00</v>
+        <v>231616</v>
       </c>
       <c r="AM49" t="s">
         <v>177</v>
@@ -7607,7 +7989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:46">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -7633,34 +8015,34 @@
         <v>7</v>
       </c>
       <c r="I50" s="2">
-        <v>12102.000</v>
+        <v>12102</v>
       </c>
       <c r="J50" s="2">
-        <v>19363.200</v>
+        <v>19363.2</v>
       </c>
       <c r="K50" s="2">
-        <v>5754.000</v>
+        <v>5754</v>
       </c>
       <c r="L50" s="2">
-        <v>9206.400</v>
+        <v>9206.4</v>
       </c>
       <c r="M50" s="2">
-        <v>6348.000</v>
+        <v>6348</v>
       </c>
       <c r="N50" s="2">
-        <v>10156.800</v>
+        <v>10156.799999999999</v>
       </c>
       <c r="O50" s="2">
-        <v>2478.000</v>
+        <v>2478</v>
       </c>
       <c r="P50" s="2">
-        <v>3964.800</v>
+        <v>3964.8</v>
       </c>
       <c r="Q50" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R50" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S50" s="4">
         <v>43705</v>
@@ -7745,7 +8127,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:46">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -7771,34 +8153,34 @@
         <v>7</v>
       </c>
       <c r="I51" s="2">
-        <v>5507.000</v>
+        <v>5507</v>
       </c>
       <c r="J51" s="2">
-        <v>6424.833</v>
+        <v>6424.8329999999996</v>
       </c>
       <c r="K51" s="2">
-        <v>4967.000</v>
+        <v>4967</v>
       </c>
       <c r="L51" s="2">
-        <v>5794.833</v>
+        <v>5794.8329999999996</v>
       </c>
       <c r="M51" s="2">
-        <v>540.000</v>
+        <v>540</v>
       </c>
       <c r="N51" s="2">
-        <v>630.000</v>
+        <v>630</v>
       </c>
       <c r="O51" s="2">
-        <v>4967.000</v>
+        <v>4967</v>
       </c>
       <c r="P51" s="2">
-        <v>5794.833</v>
+        <v>5794.8329999999996</v>
       </c>
       <c r="Q51" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R51" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S51" s="4">
         <v>43706</v>
@@ -7883,7 +8265,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:46">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -7909,34 +8291,34 @@
         <v>7</v>
       </c>
       <c r="I52" s="2">
-        <v>13026.000</v>
+        <v>13026</v>
       </c>
       <c r="J52" s="2">
-        <v>8684.000</v>
+        <v>8684</v>
       </c>
       <c r="K52" s="2">
-        <v>10572.000</v>
+        <v>10572</v>
       </c>
       <c r="L52" s="2">
-        <v>7048.000</v>
+        <v>7048</v>
       </c>
       <c r="M52" s="2">
-        <v>2454.000</v>
+        <v>2454</v>
       </c>
       <c r="N52" s="2">
-        <v>1636.000</v>
+        <v>1636</v>
       </c>
       <c r="O52" s="2">
-        <v>1026.000</v>
+        <v>1026</v>
       </c>
       <c r="P52" s="2">
-        <v>684.000</v>
+        <v>684</v>
       </c>
       <c r="Q52" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R52" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S52" s="4">
         <v>43712</v>
@@ -8021,7 +8403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:46">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -8047,34 +8429,34 @@
         <v>7</v>
       </c>
       <c r="I53" s="2">
-        <v>4250.000</v>
+        <v>4250</v>
       </c>
       <c r="J53" s="2">
-        <v>5666.667</v>
+        <v>5666.6670000000004</v>
       </c>
       <c r="K53" s="2">
-        <v>4192.000</v>
+        <v>4192</v>
       </c>
       <c r="L53" s="2">
-        <v>5589.333</v>
+        <v>5589.3329999999996</v>
       </c>
       <c r="M53" s="2">
-        <v>58.000</v>
+        <v>58</v>
       </c>
       <c r="N53" s="2">
-        <v>77.334</v>
+        <v>77.334000000000003</v>
       </c>
       <c r="O53" s="2">
-        <v>4192.000</v>
+        <v>4192</v>
       </c>
       <c r="P53" s="2">
-        <v>5589.333</v>
+        <v>5589.3329999999996</v>
       </c>
       <c r="Q53" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R53" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S53" s="4">
         <v>43714</v>
@@ -8132,7 +8514,7 @@
         <v>97</v>
       </c>
       <c r="AL53" s="5">
-        <v>943627.50</v>
+        <v>943627.5</v>
       </c>
       <c r="AM53" t="s">
         <v>194</v>
@@ -8159,7 +8541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:46">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -8185,34 +8567,34 @@
         <v>7</v>
       </c>
       <c r="I54" s="2">
-        <v>17500.000</v>
+        <v>17500</v>
       </c>
       <c r="J54" s="2">
-        <v>23333.333</v>
+        <v>23333.332999999999</v>
       </c>
       <c r="K54" s="2">
-        <v>11380.000</v>
+        <v>11380</v>
       </c>
       <c r="L54" s="2">
-        <v>15173.333</v>
+        <v>15173.333000000001</v>
       </c>
       <c r="M54" s="2">
-        <v>6120.000</v>
+        <v>6120</v>
       </c>
       <c r="N54" s="2">
-        <v>8160.000</v>
+        <v>8160</v>
       </c>
       <c r="O54" s="2">
-        <v>3780.000</v>
+        <v>3780</v>
       </c>
       <c r="P54" s="2">
-        <v>5040.000</v>
+        <v>5040</v>
       </c>
       <c r="Q54" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R54" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S54" s="4">
         <v>43714</v>
@@ -8270,7 +8652,7 @@
         <v>94</v>
       </c>
       <c r="AL54" s="5">
-        <v>3676225.00</v>
+        <v>3676225</v>
       </c>
       <c r="AM54" t="s">
         <v>196</v>
@@ -8297,7 +8679,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:46">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -8323,34 +8705,34 @@
         <v>7</v>
       </c>
       <c r="I55" s="2">
-        <v>5200.000</v>
+        <v>5200</v>
       </c>
       <c r="J55" s="2">
-        <v>6066.667</v>
+        <v>6066.6670000000004</v>
       </c>
       <c r="K55" s="2">
-        <v>4818.000</v>
+        <v>4818</v>
       </c>
       <c r="L55" s="2">
-        <v>5621.000</v>
+        <v>5621</v>
       </c>
       <c r="M55" s="2">
-        <v>382.000</v>
+        <v>382</v>
       </c>
       <c r="N55" s="2">
-        <v>445.667</v>
+        <v>445.66699999999997</v>
       </c>
       <c r="O55" s="2">
-        <v>4818.000</v>
+        <v>4818</v>
       </c>
       <c r="P55" s="2">
-        <v>5621.000</v>
+        <v>5621</v>
       </c>
       <c r="Q55" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R55" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S55" s="4">
         <v>43714</v>
@@ -8408,7 +8790,7 @@
         <v>101</v>
       </c>
       <c r="AL55" s="5">
-        <v>1094912.00</v>
+        <v>1094912</v>
       </c>
       <c r="AM55" t="s">
         <v>198</v>
@@ -8435,7 +8817,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:46">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -8461,34 +8843,34 @@
         <v>7</v>
       </c>
       <c r="I56" s="2">
-        <v>30000.000</v>
+        <v>30000</v>
       </c>
       <c r="J56" s="2">
-        <v>20000.000</v>
+        <v>20000</v>
       </c>
       <c r="K56" s="2">
-        <v>9083.000</v>
+        <v>9083</v>
       </c>
       <c r="L56" s="2">
-        <v>6055.333</v>
+        <v>6055.3329999999996</v>
       </c>
       <c r="M56" s="2">
-        <v>20917.000</v>
+        <v>20917</v>
       </c>
       <c r="N56" s="2">
-        <v>13944.667</v>
+        <v>13944.666999999999</v>
       </c>
       <c r="O56" s="2">
-        <v>9083.000</v>
+        <v>9083</v>
       </c>
       <c r="P56" s="2">
-        <v>6055.333</v>
+        <v>6055.3329999999996</v>
       </c>
       <c r="Q56" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R56" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S56" s="4">
         <v>43714</v>
@@ -8546,7 +8928,7 @@
         <v>29</v>
       </c>
       <c r="AL56" s="5">
-        <v>6363600.00</v>
+        <v>6363600</v>
       </c>
       <c r="AM56" t="s">
         <v>200</v>
@@ -8573,7 +8955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:46">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -8599,34 +8981,34 @@
         <v>7</v>
       </c>
       <c r="I57" s="2">
-        <v>30.000</v>
+        <v>30</v>
       </c>
       <c r="J57" s="2">
-        <v>20.000</v>
+        <v>20</v>
       </c>
       <c r="K57" s="2">
-        <v>30.000</v>
+        <v>30</v>
       </c>
       <c r="L57" s="2">
-        <v>20.000</v>
+        <v>20</v>
       </c>
       <c r="M57" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N57" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O57" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="P57" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="Q57" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R57" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S57" s="4">
         <v>43445</v>
@@ -8680,7 +9062,7 @@
         <v>48</v>
       </c>
       <c r="AL57" s="5">
-        <v>5845.50</v>
+        <v>5845.5</v>
       </c>
       <c r="AM57" t="s">
         <v>14</v>
@@ -8707,7 +9089,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:46">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -8733,34 +9115,34 @@
         <v>7</v>
       </c>
       <c r="I58" s="2">
-        <v>50.000</v>
+        <v>50</v>
       </c>
       <c r="J58" s="2">
-        <v>33.333</v>
+        <v>33.332999999999998</v>
       </c>
       <c r="K58" s="2">
-        <v>50.000</v>
+        <v>50</v>
       </c>
       <c r="L58" s="2">
-        <v>33.333</v>
+        <v>33.332999999999998</v>
       </c>
       <c r="M58" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N58" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O58" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="P58" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="Q58" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R58" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S58" s="4">
         <v>43558</v>
@@ -8814,7 +9196,7 @@
         <v>29</v>
       </c>
       <c r="AL58" s="5">
-        <v>10606.00</v>
+        <v>10606</v>
       </c>
       <c r="AM58" t="s">
         <v>14</v>
@@ -8841,7 +9223,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:46">
+    <row r="59" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -8867,34 +9249,34 @@
         <v>7</v>
       </c>
       <c r="I59" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="J59" s="2">
-        <v>0.667</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="K59" s="2">
-        <v>1.000</v>
+        <v>1</v>
       </c>
       <c r="L59" s="2">
-        <v>0.667</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="M59" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="N59" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="O59" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="P59" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="Q59" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="R59" s="3">
-        <v>0.000</v>
+        <v>0</v>
       </c>
       <c r="S59" s="4">
         <v>43696</v>

</xml_diff>